<commit_message>
Revert "Stereometrie - procvičení"
This reverts commit a3b54143c49450c6fa553c22ede27a053dd84754.
</commit_message>
<xml_diff>
--- a/statusy.xlsx
+++ b/statusy.xlsx
@@ -1,22 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28623"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/8a2976948ab537ed/Dokumenty/Škola/Maturita/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="102" documentId="11_AD4D80C4656A4B7AC02E74E95B186FBC5BDEDD87" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{983EC7CD-2E80-4574-B3BF-06A9FF4C2647}"/>
+  <xr:revisionPtr revIDLastSave="47" documentId="11_AD4D80C4656A4B7AC02E74E95B186FBC5BDEDD87" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{0E7C4B1A-7605-4567-B485-9AD0F63B7BC5}"/>
   <bookViews>
     <workbookView xWindow="-19320" yWindow="-105" windowWidth="19440" windowHeight="14880" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ČJ" sheetId="1" r:id="rId1"/>
     <sheet name="M" sheetId="2" r:id="rId2"/>
-    <sheet name="IVT" sheetId="3" r:id="rId3"/>
-    <sheet name="F" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -28,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="157" uniqueCount="130">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="115">
   <si>
     <t>Pořadí</t>
   </si>
@@ -315,12 +313,24 @@
     <t>OK</t>
   </si>
   <si>
+    <t>bez kontextu</t>
+  </si>
+  <si>
+    <t>přečteno</t>
+  </si>
+  <si>
     <t>logika</t>
   </si>
   <si>
+    <t>TODO důkazy procvičit</t>
+  </si>
+  <si>
     <t>y</t>
   </si>
   <si>
+    <t>těžký příklady</t>
+  </si>
+  <si>
     <t>elipsa</t>
   </si>
   <si>
@@ -345,79 +355,22 @@
     <t>výrazy</t>
   </si>
   <si>
+    <t>nemá zadání</t>
+  </si>
+  <si>
     <t>vektory</t>
   </si>
   <si>
     <t>stereometrie</t>
   </si>
   <si>
+    <t>procvičit řezy, odchylky, průniky s přímkou</t>
+  </si>
+  <si>
     <t>příklady na shodnost, podobnost</t>
   </si>
   <si>
-    <t>TODO</t>
-  </si>
-  <si>
-    <t>Kontext autora</t>
-  </si>
-  <si>
-    <t>Doplnit</t>
-  </si>
-  <si>
-    <t>OK?</t>
-  </si>
-  <si>
-    <t>důkazy procvičit</t>
-  </si>
-  <si>
-    <t>posloupnosti</t>
-  </si>
-  <si>
-    <t>parabola</t>
-  </si>
-  <si>
-    <t>výpočty ploch a objemů</t>
-  </si>
-  <si>
-    <t>integrál</t>
-  </si>
-  <si>
-    <t>euklidovy věty, příklady</t>
-  </si>
-  <si>
-    <t>koule</t>
-  </si>
-  <si>
-    <t>binomické rozdělení</t>
-  </si>
-  <si>
-    <t>derivace</t>
-  </si>
-  <si>
-    <t>přímky</t>
-  </si>
-  <si>
-    <t>tvary ~ úsekový tvar</t>
-  </si>
-  <si>
-    <t>stejnolehlost</t>
-  </si>
-  <si>
-    <t>metody řešení</t>
-  </si>
-  <si>
-    <t>tvary rovnic, ekcentricity</t>
-  </si>
-  <si>
-    <t>průběh funkce - kategorie, konvexní / konkávní</t>
-  </si>
-  <si>
-    <t>vektorový součin</t>
-  </si>
-  <si>
-    <t>X zadání</t>
-  </si>
-  <si>
-    <t>(odchylky), průniky těles s přímkou</t>
+    <t>procvičit r-ce vyšších stupňů</t>
   </si>
 </sst>
 </file>
@@ -450,60 +403,12 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="10">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFF0000"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF92D050"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.39997558519241921"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="-0.249977111117893"/>
-        <bgColor indexed="64"/>
-      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -518,7 +423,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
@@ -541,17 +446,9 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normální" xfId="0" builtinId="0"/>
@@ -904,10 +801,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F29"/>
+  <dimension ref="A1:G29"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E19" sqref="E19"/>
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -918,13 +815,13 @@
     <col min="4" max="4" width="20.90625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A1" s="1"/>
       <c r="B1" s="2"/>
       <c r="C1" s="2"/>
       <c r="D1" s="3"/>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A2" s="4" t="s">
         <v>0</v>
       </c>
@@ -937,11 +834,8 @@
       <c r="D2" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="F2" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A3" s="5" t="s">
         <v>4</v>
       </c>
@@ -954,11 +848,8 @@
       <c r="D3" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="E3" s="10" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A4" s="5" t="s">
         <v>8</v>
       </c>
@@ -971,14 +862,14 @@
       <c r="D4" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="E4" t="s">
-        <v>94</v>
-      </c>
       <c r="F4" t="s">
         <v>94</v>
       </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G4" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A5" s="5" t="s">
         <v>11</v>
       </c>
@@ -991,10 +882,11 @@
       <c r="D5" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="E5" s="9"/>
-      <c r="F5" s="9"/>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="F5" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A6" s="5" t="s">
         <v>15</v>
       </c>
@@ -1008,7 +900,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A7" s="5" t="s">
         <v>18</v>
       </c>
@@ -1021,11 +913,8 @@
       <c r="D7" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="F7" s="9" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.35">
+    </row>
+    <row r="8" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A8" s="5" t="s">
         <v>22</v>
       </c>
@@ -1038,9 +927,8 @@
       <c r="D8" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="F8" s="9"/>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.35">
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A9" s="5" t="s">
         <v>25</v>
       </c>
@@ -1053,12 +941,8 @@
       <c r="D9" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="E9" s="10"/>
-      <c r="F9" s="10" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.35">
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A10" s="5" t="s">
         <v>29</v>
       </c>
@@ -1071,9 +955,8 @@
       <c r="D10" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="F10" s="10"/>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.35">
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A11" s="5" t="s">
         <v>33</v>
       </c>
@@ -1086,11 +969,8 @@
       <c r="D11" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="F11" s="10" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.35">
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A12" s="5" t="s">
         <v>37</v>
       </c>
@@ -1103,9 +983,8 @@
       <c r="D12" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="F12" s="9"/>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.35">
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A13" s="5" t="s">
         <v>41</v>
       </c>
@@ -1118,11 +997,8 @@
       <c r="D13" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="F13" s="9" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.35">
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A14" s="5" t="s">
         <v>44</v>
       </c>
@@ -1135,9 +1011,8 @@
       <c r="D14" s="7" t="s">
         <v>47</v>
       </c>
-      <c r="F14" s="9"/>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.35">
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A15" s="5" t="s">
         <v>48</v>
       </c>
@@ -1150,9 +1025,8 @@
       <c r="D15" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="F15" s="9"/>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.35">
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A16" s="5" t="s">
         <v>51</v>
       </c>
@@ -1165,9 +1039,8 @@
       <c r="D16" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="F16" s="9"/>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.35">
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A17" s="5" t="s">
         <v>55</v>
       </c>
@@ -1180,9 +1053,8 @@
       <c r="D17" s="3" t="s">
         <v>57</v>
       </c>
-      <c r="F17" s="9"/>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.35">
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A18" s="5" t="s">
         <v>58</v>
       </c>
@@ -1195,11 +1067,8 @@
       <c r="D18" s="3" t="s">
         <v>61</v>
       </c>
-      <c r="F18" s="10" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.35">
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A19" s="5" t="s">
         <v>62</v>
       </c>
@@ -1212,14 +1081,8 @@
       <c r="D19" s="3" t="s">
         <v>65</v>
       </c>
-      <c r="E19" s="8" t="s">
-        <v>108</v>
-      </c>
-      <c r="F19" s="10" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.35">
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A20" s="5" t="s">
         <v>66</v>
       </c>
@@ -1232,9 +1095,8 @@
       <c r="D20" s="3" t="s">
         <v>68</v>
       </c>
-      <c r="F20" s="9"/>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.35">
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A21" s="5" t="s">
         <v>69</v>
       </c>
@@ -1247,9 +1109,8 @@
       <c r="D21" s="3" t="s">
         <v>72</v>
       </c>
-      <c r="F21" s="9"/>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.35">
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A22" s="5" t="s">
         <v>73</v>
       </c>
@@ -1262,11 +1123,8 @@
       <c r="D22" s="3" t="s">
         <v>75</v>
       </c>
-      <c r="F22" s="9" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.35">
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A23" s="5" t="s">
         <v>76</v>
       </c>
@@ -1279,11 +1137,8 @@
       <c r="D23" s="3" t="s">
         <v>79</v>
       </c>
-      <c r="F23" s="10" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.35">
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A24" s="5" t="s">
         <v>80</v>
       </c>
@@ -1296,11 +1151,8 @@
       <c r="D24" s="3" t="s">
         <v>83</v>
       </c>
-      <c r="F24" s="9" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.35">
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A25" s="5" t="s">
         <v>84</v>
       </c>
@@ -1313,9 +1165,8 @@
       <c r="D25" s="3" t="s">
         <v>86</v>
       </c>
-      <c r="F25" s="9"/>
-    </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.35">
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A26" s="5" t="s">
         <v>87</v>
       </c>
@@ -1328,11 +1179,8 @@
       <c r="D26" s="3" t="s">
         <v>90</v>
       </c>
-      <c r="F26" s="9" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.35">
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A27" s="5" t="s">
         <v>91</v>
       </c>
@@ -1345,17 +1193,16 @@
       <c r="D27" s="3" t="s">
         <v>93</v>
       </c>
-      <c r="F27" s="9"/>
-    </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.35">
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A28" s="5"/>
       <c r="B28" s="6"/>
       <c r="C28" s="2"/>
       <c r="D28" s="3"/>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A29" s="11"/>
-      <c r="B29" s="11"/>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A29" s="8"/>
+      <c r="B29" s="8"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -1376,10 +1223,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6888E1A3-AFF6-435D-BF5D-FC71C033C81E}">
-  <dimension ref="B2:E26"/>
+  <dimension ref="B2:D26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D20" sqref="D20"/>
+      <selection activeCell="K26" sqref="K26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1387,283 +1234,204 @@
     <col min="3" max="3" width="16.7265625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="2" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B2">
         <v>1</v>
       </c>
       <c r="C2" t="s">
-        <v>96</v>
-      </c>
-      <c r="D2" s="13" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="3" spans="2:5" x14ac:dyDescent="0.35">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="3" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B3">
         <v>2</v>
       </c>
       <c r="C3" t="s">
-        <v>96</v>
-      </c>
-      <c r="D3" s="13"/>
-    </row>
-    <row r="4" spans="2:5" x14ac:dyDescent="0.35">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="4" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B4">
         <v>3</v>
       </c>
       <c r="C4" t="s">
-        <v>96</v>
-      </c>
-      <c r="D4" s="13"/>
-    </row>
-    <row r="5" spans="2:5" x14ac:dyDescent="0.35">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="5" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B5">
         <v>4</v>
       </c>
       <c r="C5" t="s">
-        <v>96</v>
-      </c>
-      <c r="D5" s="13"/>
-    </row>
-    <row r="6" spans="2:5" x14ac:dyDescent="0.35">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="6" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B6">
         <v>5</v>
       </c>
       <c r="C6" t="s">
-        <v>96</v>
-      </c>
-      <c r="D6" s="13"/>
-    </row>
-    <row r="7" spans="2:5" x14ac:dyDescent="0.35">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="7" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B7">
         <v>6</v>
       </c>
       <c r="C7" t="s">
-        <v>96</v>
-      </c>
-      <c r="D7" s="13"/>
-    </row>
-    <row r="8" spans="2:5" x14ac:dyDescent="0.35">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="8" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B8">
         <v>7</v>
       </c>
       <c r="C8" t="s">
-        <v>100</v>
-      </c>
-      <c r="D8" s="13"/>
-      <c r="E8" s="14" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="9" spans="2:5" x14ac:dyDescent="0.35">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="9" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B9">
         <v>8</v>
       </c>
       <c r="C9" t="s">
-        <v>104</v>
-      </c>
-      <c r="D9" s="13"/>
-    </row>
-    <row r="10" spans="2:5" x14ac:dyDescent="0.35">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="10" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B10">
         <v>9</v>
       </c>
       <c r="C10" t="s">
-        <v>95</v>
-      </c>
-      <c r="D10" s="13" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="11" spans="2:5" x14ac:dyDescent="0.35">
+        <v>97</v>
+      </c>
+      <c r="D10" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="11" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B11">
         <v>10</v>
       </c>
-      <c r="C11" t="s">
-        <v>113</v>
-      </c>
-      <c r="D11" s="16" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="12" spans="2:5" x14ac:dyDescent="0.35">
+    </row>
+    <row r="12" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B12">
         <v>11</v>
       </c>
       <c r="C12" t="s">
-        <v>97</v>
-      </c>
-      <c r="D12" s="13" t="s">
-        <v>99</v>
-      </c>
-      <c r="E12" s="14"/>
-    </row>
-    <row r="13" spans="2:5" x14ac:dyDescent="0.35">
+        <v>101</v>
+      </c>
+      <c r="D12" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="13" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B13">
         <v>12</v>
       </c>
-      <c r="C13" t="s">
-        <v>114</v>
-      </c>
-      <c r="D13" s="13"/>
-      <c r="E13" s="14" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="14" spans="2:5" x14ac:dyDescent="0.35">
+    </row>
+    <row r="14" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B14">
         <v>13</v>
       </c>
       <c r="C14" t="s">
-        <v>98</v>
-      </c>
-      <c r="D14" s="12" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="15" spans="2:5" x14ac:dyDescent="0.35">
+        <v>102</v>
+      </c>
+      <c r="D14" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="15" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B15">
         <v>14</v>
       </c>
       <c r="C15" t="s">
-        <v>105</v>
-      </c>
-      <c r="D15" s="13" t="s">
-        <v>128</v>
-      </c>
-      <c r="E15" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="16" spans="2:5" x14ac:dyDescent="0.35">
+        <v>110</v>
+      </c>
+      <c r="D15" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="16" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B16">
         <v>15</v>
       </c>
       <c r="C16" t="s">
-        <v>103</v>
-      </c>
-      <c r="D16" s="13"/>
+        <v>107</v>
+      </c>
     </row>
     <row r="17" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B17">
         <v>16</v>
       </c>
       <c r="C17" t="s">
-        <v>101</v>
-      </c>
-      <c r="D17" s="13" t="s">
-        <v>102</v>
+        <v>105</v>
+      </c>
+      <c r="D17" t="s">
+        <v>106</v>
       </c>
     </row>
     <row r="18" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B18">
         <v>17</v>
       </c>
-      <c r="D18" s="13" t="s">
-        <v>119</v>
-      </c>
     </row>
     <row r="19" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B19">
         <v>18</v>
       </c>
-      <c r="D19" s="13"/>
     </row>
     <row r="20" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B20">
         <v>19</v>
       </c>
       <c r="C20" t="s">
-        <v>106</v>
-      </c>
-      <c r="D20" s="15" t="s">
-        <v>129</v>
+        <v>111</v>
+      </c>
+      <c r="D20" t="s">
+        <v>112</v>
       </c>
     </row>
     <row r="21" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B21">
         <v>20</v>
       </c>
-      <c r="C21" t="s">
-        <v>120</v>
-      </c>
-      <c r="D21" s="13"/>
     </row>
     <row r="22" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B22">
         <v>21</v>
       </c>
-      <c r="C22" t="s">
-        <v>116</v>
-      </c>
-      <c r="D22" s="13" t="s">
-        <v>96</v>
-      </c>
     </row>
     <row r="23" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B23">
         <v>22</v>
       </c>
-      <c r="D23" s="12" t="s">
-        <v>117</v>
-      </c>
     </row>
     <row r="24" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B24">
         <v>23</v>
       </c>
       <c r="C24" t="s">
-        <v>121</v>
-      </c>
-      <c r="D24" s="13" t="s">
-        <v>122</v>
+        <v>99</v>
       </c>
     </row>
     <row r="25" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B25">
         <v>24</v>
       </c>
-      <c r="C25" t="s">
-        <v>123</v>
-      </c>
-      <c r="D25" s="16" t="s">
-        <v>107</v>
+      <c r="D25" t="s">
+        <v>113</v>
       </c>
     </row>
     <row r="26" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B26">
         <v>25</v>
       </c>
-      <c r="D26" s="13" t="s">
-        <v>124</v>
+      <c r="D26" t="s">
+        <v>114</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A11C67C3-F387-4F8E-8E25-7C66B461CAAB}">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E61B2A55-D999-468E-A8C4-E81821571AAF}">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Reapply "Stereometrie - procvičení"
This reverts commit 72e5507e8cf8af6a1dd4ce8ac3f40d62cbc99618.
</commit_message>
<xml_diff>
--- a/statusy.xlsx
+++ b/statusy.xlsx
@@ -1,20 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28623"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28730"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/8a2976948ab537ed/Dokumenty/Škola/Maturita/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="47" documentId="11_AD4D80C4656A4B7AC02E74E95B186FBC5BDEDD87" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{0E7C4B1A-7605-4567-B485-9AD0F63B7BC5}"/>
+  <xr:revisionPtr revIDLastSave="102" documentId="11_AD4D80C4656A4B7AC02E74E95B186FBC5BDEDD87" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{983EC7CD-2E80-4574-B3BF-06A9FF4C2647}"/>
   <bookViews>
     <workbookView xWindow="-19320" yWindow="-105" windowWidth="19440" windowHeight="14880" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ČJ" sheetId="1" r:id="rId1"/>
     <sheet name="M" sheetId="2" r:id="rId2"/>
+    <sheet name="IVT" sheetId="3" r:id="rId3"/>
+    <sheet name="F" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -26,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="115">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="157" uniqueCount="130">
   <si>
     <t>Pořadí</t>
   </si>
@@ -313,24 +315,12 @@
     <t>OK</t>
   </si>
   <si>
-    <t>bez kontextu</t>
-  </si>
-  <si>
-    <t>přečteno</t>
-  </si>
-  <si>
     <t>logika</t>
   </si>
   <si>
-    <t>TODO důkazy procvičit</t>
-  </si>
-  <si>
     <t>y</t>
   </si>
   <si>
-    <t>těžký příklady</t>
-  </si>
-  <si>
     <t>elipsa</t>
   </si>
   <si>
@@ -355,22 +345,79 @@
     <t>výrazy</t>
   </si>
   <si>
-    <t>nemá zadání</t>
-  </si>
-  <si>
     <t>vektory</t>
   </si>
   <si>
     <t>stereometrie</t>
   </si>
   <si>
-    <t>procvičit řezy, odchylky, průniky s přímkou</t>
-  </si>
-  <si>
     <t>příklady na shodnost, podobnost</t>
   </si>
   <si>
-    <t>procvičit r-ce vyšších stupňů</t>
+    <t>TODO</t>
+  </si>
+  <si>
+    <t>Kontext autora</t>
+  </si>
+  <si>
+    <t>Doplnit</t>
+  </si>
+  <si>
+    <t>OK?</t>
+  </si>
+  <si>
+    <t>důkazy procvičit</t>
+  </si>
+  <si>
+    <t>posloupnosti</t>
+  </si>
+  <si>
+    <t>parabola</t>
+  </si>
+  <si>
+    <t>výpočty ploch a objemů</t>
+  </si>
+  <si>
+    <t>integrál</t>
+  </si>
+  <si>
+    <t>euklidovy věty, příklady</t>
+  </si>
+  <si>
+    <t>koule</t>
+  </si>
+  <si>
+    <t>binomické rozdělení</t>
+  </si>
+  <si>
+    <t>derivace</t>
+  </si>
+  <si>
+    <t>přímky</t>
+  </si>
+  <si>
+    <t>tvary ~ úsekový tvar</t>
+  </si>
+  <si>
+    <t>stejnolehlost</t>
+  </si>
+  <si>
+    <t>metody řešení</t>
+  </si>
+  <si>
+    <t>tvary rovnic, ekcentricity</t>
+  </si>
+  <si>
+    <t>průběh funkce - kategorie, konvexní / konkávní</t>
+  </si>
+  <si>
+    <t>vektorový součin</t>
+  </si>
+  <si>
+    <t>X zadání</t>
+  </si>
+  <si>
+    <t>(odchylky), průniky těles s přímkou</t>
   </si>
 </sst>
 </file>
@@ -403,12 +450,60 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="10">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -423,7 +518,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
@@ -446,9 +541,17 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normální" xfId="0" builtinId="0"/>
@@ -801,10 +904,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G29"/>
+  <dimension ref="A1:F29"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+      <selection activeCell="E19" sqref="E19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -815,13 +918,13 @@
     <col min="4" max="4" width="20.90625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A1" s="1"/>
       <c r="B1" s="2"/>
       <c r="C1" s="2"/>
       <c r="D1" s="3"/>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A2" s="4" t="s">
         <v>0</v>
       </c>
@@ -834,8 +937,11 @@
       <c r="D2" s="3" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="F2" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A3" s="5" t="s">
         <v>4</v>
       </c>
@@ -848,8 +954,11 @@
       <c r="D3" s="3" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="E3" s="10" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A4" s="5" t="s">
         <v>8</v>
       </c>
@@ -862,14 +971,14 @@
       <c r="D4" s="3" t="s">
         <v>10</v>
       </c>
+      <c r="E4" t="s">
+        <v>94</v>
+      </c>
       <c r="F4" t="s">
         <v>94</v>
       </c>
-      <c r="G4" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A5" s="5" t="s">
         <v>11</v>
       </c>
@@ -882,11 +991,10 @@
       <c r="D5" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="F5" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="E5" s="9"/>
+      <c r="F5" s="9"/>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A6" s="5" t="s">
         <v>15</v>
       </c>
@@ -900,7 +1008,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A7" s="5" t="s">
         <v>18</v>
       </c>
@@ -913,8 +1021,11 @@
       <c r="D7" s="3" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="8" spans="1:7" ht="29" x14ac:dyDescent="0.35">
+      <c r="F7" s="9" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A8" s="5" t="s">
         <v>22</v>
       </c>
@@ -927,8 +1038,9 @@
       <c r="D8" s="3" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="F8" s="9"/>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A9" s="5" t="s">
         <v>25</v>
       </c>
@@ -941,8 +1053,12 @@
       <c r="D9" s="3" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="E9" s="10"/>
+      <c r="F9" s="10" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A10" s="5" t="s">
         <v>29</v>
       </c>
@@ -955,8 +1071,9 @@
       <c r="D10" s="3" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="F10" s="10"/>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A11" s="5" t="s">
         <v>33</v>
       </c>
@@ -969,8 +1086,11 @@
       <c r="D11" s="3" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="F11" s="10" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A12" s="5" t="s">
         <v>37</v>
       </c>
@@ -983,8 +1103,9 @@
       <c r="D12" s="3" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="F12" s="9"/>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A13" s="5" t="s">
         <v>41</v>
       </c>
@@ -997,8 +1118,11 @@
       <c r="D13" s="3" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="F13" s="9" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A14" s="5" t="s">
         <v>44</v>
       </c>
@@ -1011,8 +1135,9 @@
       <c r="D14" s="7" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="F14" s="9"/>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A15" s="5" t="s">
         <v>48</v>
       </c>
@@ -1025,8 +1150,9 @@
       <c r="D15" s="3" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="F15" s="9"/>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A16" s="5" t="s">
         <v>51</v>
       </c>
@@ -1039,8 +1165,9 @@
       <c r="D16" s="3" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="F16" s="9"/>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A17" s="5" t="s">
         <v>55</v>
       </c>
@@ -1053,8 +1180,9 @@
       <c r="D17" s="3" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="F17" s="9"/>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A18" s="5" t="s">
         <v>58</v>
       </c>
@@ -1067,8 +1195,11 @@
       <c r="D18" s="3" t="s">
         <v>61</v>
       </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="F18" s="10" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A19" s="5" t="s">
         <v>62</v>
       </c>
@@ -1081,8 +1212,14 @@
       <c r="D19" s="3" t="s">
         <v>65</v>
       </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E19" s="8" t="s">
+        <v>108</v>
+      </c>
+      <c r="F19" s="10" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A20" s="5" t="s">
         <v>66</v>
       </c>
@@ -1095,8 +1232,9 @@
       <c r="D20" s="3" t="s">
         <v>68</v>
       </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="F20" s="9"/>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A21" s="5" t="s">
         <v>69</v>
       </c>
@@ -1109,8 +1247,9 @@
       <c r="D21" s="3" t="s">
         <v>72</v>
       </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="F21" s="9"/>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A22" s="5" t="s">
         <v>73</v>
       </c>
@@ -1123,8 +1262,11 @@
       <c r="D22" s="3" t="s">
         <v>75</v>
       </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="F22" s="9" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A23" s="5" t="s">
         <v>76</v>
       </c>
@@ -1137,8 +1279,11 @@
       <c r="D23" s="3" t="s">
         <v>79</v>
       </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="F23" s="10" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A24" s="5" t="s">
         <v>80</v>
       </c>
@@ -1151,8 +1296,11 @@
       <c r="D24" s="3" t="s">
         <v>83</v>
       </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="F24" s="9" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A25" s="5" t="s">
         <v>84</v>
       </c>
@@ -1165,8 +1313,9 @@
       <c r="D25" s="3" t="s">
         <v>86</v>
       </c>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="F25" s="9"/>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A26" s="5" t="s">
         <v>87</v>
       </c>
@@ -1179,8 +1328,11 @@
       <c r="D26" s="3" t="s">
         <v>90</v>
       </c>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="F26" s="9" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A27" s="5" t="s">
         <v>91</v>
       </c>
@@ -1193,16 +1345,17 @@
       <c r="D27" s="3" t="s">
         <v>93</v>
       </c>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="F27" s="9"/>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A28" s="5"/>
       <c r="B28" s="6"/>
       <c r="C28" s="2"/>
       <c r="D28" s="3"/>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A29" s="8"/>
-      <c r="B29" s="8"/>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A29" s="11"/>
+      <c r="B29" s="11"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -1223,10 +1376,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6888E1A3-AFF6-435D-BF5D-FC71C033C81E}">
-  <dimension ref="B2:D26"/>
+  <dimension ref="B2:E26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K26" sqref="K26"/>
+      <selection activeCell="D20" sqref="D20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1234,204 +1387,283 @@
     <col min="3" max="3" width="16.7265625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="2" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B2">
         <v>1</v>
       </c>
       <c r="C2" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="3" spans="2:4" x14ac:dyDescent="0.35">
+        <v>96</v>
+      </c>
+      <c r="D2" s="13" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="3" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B3">
         <v>2</v>
       </c>
       <c r="C3" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="4" spans="2:4" x14ac:dyDescent="0.35">
+        <v>96</v>
+      </c>
+      <c r="D3" s="13"/>
+    </row>
+    <row r="4" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B4">
         <v>3</v>
       </c>
       <c r="C4" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="5" spans="2:4" x14ac:dyDescent="0.35">
+        <v>96</v>
+      </c>
+      <c r="D4" s="13"/>
+    </row>
+    <row r="5" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B5">
         <v>4</v>
       </c>
       <c r="C5" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="6" spans="2:4" x14ac:dyDescent="0.35">
+        <v>96</v>
+      </c>
+      <c r="D5" s="13"/>
+    </row>
+    <row r="6" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B6">
         <v>5</v>
       </c>
       <c r="C6" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="7" spans="2:4" x14ac:dyDescent="0.35">
+        <v>96</v>
+      </c>
+      <c r="D6" s="13"/>
+    </row>
+    <row r="7" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B7">
         <v>6</v>
       </c>
       <c r="C7" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="8" spans="2:4" x14ac:dyDescent="0.35">
+        <v>96</v>
+      </c>
+      <c r="D7" s="13"/>
+    </row>
+    <row r="8" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B8">
         <v>7</v>
       </c>
       <c r="C8" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="9" spans="2:4" x14ac:dyDescent="0.35">
+        <v>100</v>
+      </c>
+      <c r="D8" s="13"/>
+      <c r="E8" s="14" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="9" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B9">
         <v>8</v>
       </c>
       <c r="C9" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="10" spans="2:4" x14ac:dyDescent="0.35">
+        <v>104</v>
+      </c>
+      <c r="D9" s="13"/>
+    </row>
+    <row r="10" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B10">
         <v>9</v>
       </c>
       <c r="C10" t="s">
-        <v>97</v>
-      </c>
-      <c r="D10" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="11" spans="2:4" x14ac:dyDescent="0.35">
+        <v>95</v>
+      </c>
+      <c r="D10" s="13" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="11" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B11">
         <v>10</v>
       </c>
-    </row>
-    <row r="12" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="C11" t="s">
+        <v>113</v>
+      </c>
+      <c r="D11" s="16" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="12" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B12">
         <v>11</v>
       </c>
       <c r="C12" t="s">
-        <v>101</v>
-      </c>
-      <c r="D12" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="13" spans="2:4" x14ac:dyDescent="0.35">
+        <v>97</v>
+      </c>
+      <c r="D12" s="13" t="s">
+        <v>99</v>
+      </c>
+      <c r="E12" s="14"/>
+    </row>
+    <row r="13" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B13">
         <v>12</v>
       </c>
-    </row>
-    <row r="14" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="C13" t="s">
+        <v>114</v>
+      </c>
+      <c r="D13" s="13"/>
+      <c r="E13" s="14" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="14" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B14">
         <v>13</v>
       </c>
       <c r="C14" t="s">
-        <v>102</v>
-      </c>
-      <c r="D14" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="15" spans="2:4" x14ac:dyDescent="0.35">
+        <v>98</v>
+      </c>
+      <c r="D14" s="12" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="15" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B15">
         <v>14</v>
       </c>
       <c r="C15" t="s">
-        <v>110</v>
-      </c>
-      <c r="D15" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="16" spans="2:4" x14ac:dyDescent="0.35">
+        <v>105</v>
+      </c>
+      <c r="D15" s="13" t="s">
+        <v>128</v>
+      </c>
+      <c r="E15" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="16" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B16">
         <v>15</v>
       </c>
       <c r="C16" t="s">
-        <v>107</v>
-      </c>
+        <v>103</v>
+      </c>
+      <c r="D16" s="13"/>
     </row>
     <row r="17" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B17">
         <v>16</v>
       </c>
       <c r="C17" t="s">
-        <v>105</v>
-      </c>
-      <c r="D17" t="s">
-        <v>106</v>
+        <v>101</v>
+      </c>
+      <c r="D17" s="13" t="s">
+        <v>102</v>
       </c>
     </row>
     <row r="18" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B18">
         <v>17</v>
       </c>
+      <c r="D18" s="13" t="s">
+        <v>119</v>
+      </c>
     </row>
     <row r="19" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B19">
         <v>18</v>
       </c>
+      <c r="D19" s="13"/>
     </row>
     <row r="20" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B20">
         <v>19</v>
       </c>
       <c r="C20" t="s">
-        <v>111</v>
-      </c>
-      <c r="D20" t="s">
-        <v>112</v>
+        <v>106</v>
+      </c>
+      <c r="D20" s="15" t="s">
+        <v>129</v>
       </c>
     </row>
     <row r="21" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B21">
         <v>20</v>
       </c>
+      <c r="C21" t="s">
+        <v>120</v>
+      </c>
+      <c r="D21" s="13"/>
     </row>
     <row r="22" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B22">
         <v>21</v>
       </c>
+      <c r="C22" t="s">
+        <v>116</v>
+      </c>
+      <c r="D22" s="13" t="s">
+        <v>96</v>
+      </c>
     </row>
     <row r="23" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B23">
         <v>22</v>
       </c>
+      <c r="D23" s="12" t="s">
+        <v>117</v>
+      </c>
     </row>
     <row r="24" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B24">
         <v>23</v>
       </c>
       <c r="C24" t="s">
-        <v>99</v>
+        <v>121</v>
+      </c>
+      <c r="D24" s="13" t="s">
+        <v>122</v>
       </c>
     </row>
     <row r="25" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B25">
         <v>24</v>
       </c>
-      <c r="D25" t="s">
-        <v>113</v>
+      <c r="C25" t="s">
+        <v>123</v>
+      </c>
+      <c r="D25" s="16" t="s">
+        <v>107</v>
       </c>
     </row>
     <row r="26" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B26">
         <v>25</v>
       </c>
-      <c r="D26" t="s">
-        <v>114</v>
+      <c r="D26" s="13" t="s">
+        <v>124</v>
       </c>
     </row>
   </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A11C67C3-F387-4F8E-8E25-7C66B461CAAB}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E61B2A55-D999-468E-A8C4-E81821571AAF}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Oprava Statusů : //
</commit_message>
<xml_diff>
--- a/statusy.xlsx
+++ b/statusy.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/8a2976948ab537ed/Dokumenty/Škola/Maturita/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="102" documentId="11_AD4D80C4656A4B7AC02E74E95B186FBC5BDEDD87" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{983EC7CD-2E80-4574-B3BF-06A9FF4C2647}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{2CD75C1D-5E9B-443C-9A12-C63864DAEB8C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-19320" yWindow="-105" windowWidth="19440" windowHeight="14880" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ČJ" sheetId="1" r:id="rId1"/>
@@ -544,14 +544,14 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normální" xfId="0" builtinId="0"/>
@@ -906,8 +906,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F29"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E19" sqref="E19"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1354,8 +1354,8 @@
       <c r="D28" s="3"/>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A29" s="11"/>
-      <c r="B29" s="11"/>
+      <c r="A29" s="16"/>
+      <c r="B29" s="16"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -1378,7 +1378,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6888E1A3-AFF6-435D-BF5D-FC71C033C81E}">
   <dimension ref="B2:E26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D20" sqref="D20"/>
     </sheetView>
   </sheetViews>
@@ -1394,7 +1394,7 @@
       <c r="C2" t="s">
         <v>96</v>
       </c>
-      <c r="D2" s="13" t="s">
+      <c r="D2" s="12" t="s">
         <v>126</v>
       </c>
     </row>
@@ -1405,7 +1405,7 @@
       <c r="C3" t="s">
         <v>96</v>
       </c>
-      <c r="D3" s="13"/>
+      <c r="D3" s="12"/>
     </row>
     <row r="4" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B4">
@@ -1414,7 +1414,7 @@
       <c r="C4" t="s">
         <v>96</v>
       </c>
-      <c r="D4" s="13"/>
+      <c r="D4" s="12"/>
     </row>
     <row r="5" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B5">
@@ -1423,7 +1423,7 @@
       <c r="C5" t="s">
         <v>96</v>
       </c>
-      <c r="D5" s="13"/>
+      <c r="D5" s="12"/>
     </row>
     <row r="6" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B6">
@@ -1432,7 +1432,7 @@
       <c r="C6" t="s">
         <v>96</v>
       </c>
-      <c r="D6" s="13"/>
+      <c r="D6" s="12"/>
     </row>
     <row r="7" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B7">
@@ -1441,7 +1441,7 @@
       <c r="C7" t="s">
         <v>96</v>
       </c>
-      <c r="D7" s="13"/>
+      <c r="D7" s="12"/>
     </row>
     <row r="8" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B8">
@@ -1450,8 +1450,8 @@
       <c r="C8" t="s">
         <v>100</v>
       </c>
-      <c r="D8" s="13"/>
-      <c r="E8" s="14" t="s">
+      <c r="D8" s="12"/>
+      <c r="E8" s="13" t="s">
         <v>125</v>
       </c>
     </row>
@@ -1462,7 +1462,7 @@
       <c r="C9" t="s">
         <v>104</v>
       </c>
-      <c r="D9" s="13"/>
+      <c r="D9" s="12"/>
     </row>
     <row r="10" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B10">
@@ -1471,7 +1471,7 @@
       <c r="C10" t="s">
         <v>95</v>
       </c>
-      <c r="D10" s="13" t="s">
+      <c r="D10" s="12" t="s">
         <v>112</v>
       </c>
     </row>
@@ -1482,7 +1482,7 @@
       <c r="C11" t="s">
         <v>113</v>
       </c>
-      <c r="D11" s="16" t="s">
+      <c r="D11" s="15" t="s">
         <v>96</v>
       </c>
     </row>
@@ -1493,10 +1493,10 @@
       <c r="C12" t="s">
         <v>97</v>
       </c>
-      <c r="D12" s="13" t="s">
+      <c r="D12" s="12" t="s">
         <v>99</v>
       </c>
-      <c r="E12" s="14"/>
+      <c r="E12" s="13"/>
     </row>
     <row r="13" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B13">
@@ -1505,8 +1505,8 @@
       <c r="C13" t="s">
         <v>114</v>
       </c>
-      <c r="D13" s="13"/>
-      <c r="E13" s="14" t="s">
+      <c r="D13" s="12"/>
+      <c r="E13" s="13" t="s">
         <v>115</v>
       </c>
     </row>
@@ -1517,7 +1517,7 @@
       <c r="C14" t="s">
         <v>98</v>
       </c>
-      <c r="D14" s="12" t="s">
+      <c r="D14" s="11" t="s">
         <v>118</v>
       </c>
     </row>
@@ -1528,7 +1528,7 @@
       <c r="C15" t="s">
         <v>105</v>
       </c>
-      <c r="D15" s="13" t="s">
+      <c r="D15" s="12" t="s">
         <v>128</v>
       </c>
       <c r="E15" t="s">
@@ -1542,7 +1542,7 @@
       <c r="C16" t="s">
         <v>103</v>
       </c>
-      <c r="D16" s="13"/>
+      <c r="D16" s="12"/>
     </row>
     <row r="17" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B17">
@@ -1551,7 +1551,7 @@
       <c r="C17" t="s">
         <v>101</v>
       </c>
-      <c r="D17" s="13" t="s">
+      <c r="D17" s="12" t="s">
         <v>102</v>
       </c>
     </row>
@@ -1559,7 +1559,7 @@
       <c r="B18">
         <v>17</v>
       </c>
-      <c r="D18" s="13" t="s">
+      <c r="D18" s="12" t="s">
         <v>119</v>
       </c>
     </row>
@@ -1567,7 +1567,7 @@
       <c r="B19">
         <v>18</v>
       </c>
-      <c r="D19" s="13"/>
+      <c r="D19" s="12"/>
     </row>
     <row r="20" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B20">
@@ -1576,7 +1576,7 @@
       <c r="C20" t="s">
         <v>106</v>
       </c>
-      <c r="D20" s="15" t="s">
+      <c r="D20" s="14" t="s">
         <v>129</v>
       </c>
     </row>
@@ -1587,7 +1587,7 @@
       <c r="C21" t="s">
         <v>120</v>
       </c>
-      <c r="D21" s="13"/>
+      <c r="D21" s="12"/>
     </row>
     <row r="22" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B22">
@@ -1596,7 +1596,7 @@
       <c r="C22" t="s">
         <v>116</v>
       </c>
-      <c r="D22" s="13" t="s">
+      <c r="D22" s="12" t="s">
         <v>96</v>
       </c>
     </row>
@@ -1604,7 +1604,7 @@
       <c r="B23">
         <v>22</v>
       </c>
-      <c r="D23" s="12" t="s">
+      <c r="D23" s="11" t="s">
         <v>117</v>
       </c>
     </row>
@@ -1615,7 +1615,7 @@
       <c r="C24" t="s">
         <v>121</v>
       </c>
-      <c r="D24" s="13" t="s">
+      <c r="D24" s="12" t="s">
         <v>122</v>
       </c>
     </row>
@@ -1626,7 +1626,7 @@
       <c r="C25" t="s">
         <v>123</v>
       </c>
-      <c r="D25" s="16" t="s">
+      <c r="D25" s="15" t="s">
         <v>107</v>
       </c>
     </row>
@@ -1634,7 +1634,7 @@
       <c r="B26">
         <v>25</v>
       </c>
-      <c r="D26" s="13" t="s">
+      <c r="D26" s="12" t="s">
         <v>124</v>
       </c>
     </row>

</xml_diff>